<commit_message>
add option to see all errors of all categories for a sample
</commit_message>
<xml_diff>
--- a/tests/resources/EVA_Submission_test.xlsx
+++ b/tests/resources/EVA_Submission_test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="PLEASE READ FIRST" sheetId="1" state="visible" r:id="rId3"/>
@@ -686,7 +686,7 @@
     <t xml:space="preserve">Template Basic Details</t>
   </si>
   <si>
-    <t xml:space="preserve">Sample Name</t>
+    <t xml:space="preserve">BioSample Name</t>
   </si>
   <si>
     <t xml:space="preserve">Unique sample identifier (e.g. st-ssff31)</t>
@@ -5573,7 +5573,7 @@
   </sheetPr>
   <dimension ref="A1:O1004"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -9741,8 +9741,8 @@
   </sheetPr>
   <dimension ref="A1:B56"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10176,7 +10176,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="IrtVTf7xUCmZBNRcjFMvaCyEJlvTB6oNqXh6XCTcGZac6l0HOs2PvYrIVUVf+JnmYqRLN7+7d4uhcaWbDdElXg==" saltValue="Kwd+oWgMyKFzDZZ5ZDzrwQ==" spinCount="100000" sheet="true" objects="true" scenarios="true"/>
+  <sheetProtection sheet="true" password="e50b" objects="true" scenarios="true"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -10195,7 +10195,7 @@
   <dimension ref="A1:AS1007"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
remove sample schemas besides ERC000011
</commit_message>
<xml_diff>
--- a/tests/resources/EVA_Submission_test.xlsx
+++ b/tests/resources/EVA_Submission_test.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="584">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="584">
   <si>
     <t xml:space="preserve">PLEASE READ FIRST</t>
   </si>
@@ -905,6 +905,9 @@
     <t xml:space="preserve">2021-03-12</t>
   </si>
   <si>
+    <t xml:space="preserve">Afghanistan</t>
+  </si>
+  <si>
     <t xml:space="preserve">Alias of the analysis that produced the file. The Analysis Alias field must be the same in the following sheets: Analysis, Sample and Files.</t>
   </si>
   <si>
@@ -924,9 +927,6 @@
   </si>
   <si>
     <t xml:space="preserve">Sample(s)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Afghanistan</t>
   </si>
   <si>
     <t xml:space="preserve">454 GS</t>
@@ -2401,7 +2401,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="82">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2430,7 +2430,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2591,10 +2591,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2990,7 +2986,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="61.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="83.5"/>
@@ -3232,7 +3228,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.33"/>
@@ -3243,7 +3239,7 @@
         <v>71</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3251,7 +3247,7 @@
         <v>98</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3259,7 +3255,7 @@
         <v>105</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3267,7 +3263,7 @@
         <v>107</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6290,10 +6286,10 @@
   <dimension ref="A1:F286"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="39"/>
@@ -6301,11 +6297,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="25"/>
   </cols>
   <sheetData>
-    <row r="1" s="51" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="80" t="s">
-        <v>234</v>
-      </c>
-      <c r="D1" s="80" t="s">
+    <row r="1" s="50" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="79" t="s">
+        <v>235</v>
+      </c>
+      <c r="D1" s="79" t="s">
         <v>16</v>
       </c>
     </row>
@@ -6328,7 +6324,7 @@
         <v>225</v>
       </c>
       <c r="B3" s="40" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>100</v>
@@ -6336,7 +6332,7 @@
       <c r="E3" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="F3" s="81"/>
+      <c r="F3" s="80"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -6795,7 +6791,7 @@
       <c r="B55" s="40" t="s">
         <v>352</v>
       </c>
-      <c r="E55" s="51"/>
+      <c r="E55" s="50"/>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="40" t="s">
@@ -7933,22 +7929,22 @@
       </c>
     </row>
     <row r="283" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B283" s="82" t="s">
+      <c r="B283" s="81" t="s">
         <v>580</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B284" s="82" t="s">
+      <c r="B284" s="81" t="s">
         <v>581</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B285" s="82" t="s">
+      <c r="B285" s="81" t="s">
         <v>582</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B286" s="82" t="s">
+      <c r="B286" s="81" t="s">
         <v>583</v>
       </c>
     </row>
@@ -7975,7 +7971,7 @@
       <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.33"/>
@@ -8071,7 +8067,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="176.66"/>
@@ -8204,7 +8200,7 @@
       <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="54.5"/>
@@ -8314,7 +8310,7 @@
       <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="164.83"/>
@@ -8404,7 +8400,7 @@
       <c r="A11" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>87</v>
       </c>
     </row>
@@ -8412,7 +8408,7 @@
       <c r="A12" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>89</v>
       </c>
     </row>
@@ -8480,7 +8476,7 @@
       <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.51"/>
@@ -16647,7 +16643,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="44.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="215"/>
@@ -16702,17 +16698,17 @@
       <c r="A8" s="47" t="s">
         <v>115</v>
       </c>
-      <c r="B8" s="48" t="s">
+      <c r="B8" s="44" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="49" t="s">
+      <c r="A9" s="48" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="50" t="s">
+      <c r="A10" s="49" t="s">
         <v>118</v>
       </c>
     </row>
@@ -16765,7 +16761,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="51" t="s">
+      <c r="A17" s="50" t="s">
         <v>130</v>
       </c>
       <c r="B17" s="44"/>
@@ -16774,7 +16770,7 @@
       <c r="A18" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="52" t="s">
+      <c r="B18" s="51" t="s">
         <v>131</v>
       </c>
     </row>
@@ -16795,7 +16791,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="51" t="s">
+      <c r="A21" s="50" t="s">
         <v>136</v>
       </c>
       <c r="B21" s="44"/>
@@ -16825,7 +16821,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="51" t="s">
+      <c r="A25" s="50" t="s">
         <v>143</v>
       </c>
       <c r="B25" s="44"/>
@@ -16871,7 +16867,7 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="51" t="s">
+      <c r="A31" s="50" t="s">
         <v>154</v>
       </c>
       <c r="B31" s="44"/>
@@ -16901,7 +16897,7 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="51" t="s">
+      <c r="A35" s="50" t="s">
         <v>161</v>
       </c>
       <c r="B35" s="44"/>
@@ -16982,12 +16978,12 @@
       <c r="A45" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B45" s="52" t="s">
+      <c r="B45" s="51" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="51" t="s">
+      <c r="A46" s="50" t="s">
         <v>182</v>
       </c>
       <c r="B46" s="44"/>
@@ -17073,7 +17069,7 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="51" t="s">
+      <c r="A57" s="50" t="s">
         <v>203</v>
       </c>
       <c r="B57" s="44"/>
@@ -17085,7 +17081,7 @@
       <c r="B58" s="44"/>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="53" t="s">
+      <c r="A59" s="52" t="s">
         <v>205</v>
       </c>
       <c r="B59" s="44"/>
@@ -17117,17 +17113,17 @@
   </sheetPr>
   <dimension ref="A1:AT1003"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="R1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AB13" activeCellId="0" sqref="AB13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="54" width="5.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="53" width="5.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="54" width="5.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="53" width="5.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="21.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="36.5"/>
@@ -17147,255 +17143,255 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="54" t="s">
         <v>208</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="57" t="s">
+      <c r="B1" s="54"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="56" t="s">
         <v>209</v>
       </c>
-      <c r="E1" s="56" t="s">
+      <c r="E1" s="55" t="s">
         <v>210</v>
       </c>
-      <c r="F1" s="57" t="s">
+      <c r="F1" s="56" t="s">
         <v>211</v>
       </c>
-      <c r="G1" s="58"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
-      <c r="N1" s="59"/>
-      <c r="O1" s="60"/>
-      <c r="P1" s="60"/>
-      <c r="Q1" s="60"/>
-      <c r="R1" s="60"/>
-      <c r="S1" s="60"/>
-      <c r="T1" s="60"/>
-      <c r="U1" s="60"/>
-      <c r="V1" s="60"/>
-      <c r="W1" s="60"/>
-      <c r="X1" s="60"/>
-      <c r="Y1" s="60"/>
-      <c r="Z1" s="60"/>
-      <c r="AA1" s="61"/>
-      <c r="AB1" s="60"/>
-      <c r="AC1" s="60"/>
-      <c r="AD1" s="60"/>
-      <c r="AE1" s="60"/>
-      <c r="AF1" s="60"/>
-      <c r="AG1" s="60"/>
-      <c r="AH1" s="60"/>
-      <c r="AI1" s="60"/>
-      <c r="AJ1" s="60"/>
-      <c r="AK1" s="60"/>
-      <c r="AL1" s="60"/>
-      <c r="AM1" s="60"/>
-      <c r="AN1" s="60"/>
-      <c r="AO1" s="60"/>
-      <c r="AP1" s="60"/>
-      <c r="AQ1" s="60"/>
-      <c r="AR1" s="60"/>
-      <c r="AS1" s="60"/>
-      <c r="AT1" s="62"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="59"/>
+      <c r="S1" s="59"/>
+      <c r="T1" s="59"/>
+      <c r="U1" s="59"/>
+      <c r="V1" s="59"/>
+      <c r="W1" s="59"/>
+      <c r="X1" s="59"/>
+      <c r="Y1" s="59"/>
+      <c r="Z1" s="59"/>
+      <c r="AA1" s="60"/>
+      <c r="AB1" s="59"/>
+      <c r="AC1" s="59"/>
+      <c r="AD1" s="59"/>
+      <c r="AE1" s="59"/>
+      <c r="AF1" s="59"/>
+      <c r="AG1" s="59"/>
+      <c r="AH1" s="59"/>
+      <c r="AI1" s="59"/>
+      <c r="AJ1" s="59"/>
+      <c r="AK1" s="59"/>
+      <c r="AL1" s="59"/>
+      <c r="AM1" s="59"/>
+      <c r="AN1" s="59"/>
+      <c r="AO1" s="59"/>
+      <c r="AP1" s="59"/>
+      <c r="AQ1" s="59"/>
+      <c r="AR1" s="59"/>
+      <c r="AS1" s="59"/>
+      <c r="AT1" s="61"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="63"/>
-      <c r="B2" s="64"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="66" t="s">
+      <c r="A2" s="62"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="65" t="s">
         <v>118</v>
       </c>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="66"/>
-      <c r="K2" s="66"/>
-      <c r="L2" s="67" t="s">
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="65"/>
+      <c r="L2" s="66" t="s">
         <v>130</v>
       </c>
-      <c r="M2" s="67"/>
-      <c r="N2" s="67"/>
-      <c r="O2" s="67" t="s">
+      <c r="M2" s="66"/>
+      <c r="N2" s="66"/>
+      <c r="O2" s="66" t="s">
         <v>136</v>
       </c>
-      <c r="P2" s="67"/>
-      <c r="Q2" s="67"/>
-      <c r="R2" s="66" t="s">
+      <c r="P2" s="66"/>
+      <c r="Q2" s="66"/>
+      <c r="R2" s="65" t="s">
         <v>143</v>
       </c>
-      <c r="S2" s="66"/>
-      <c r="T2" s="66"/>
-      <c r="U2" s="66"/>
-      <c r="V2" s="66"/>
-      <c r="W2" s="66" t="s">
+      <c r="S2" s="65"/>
+      <c r="T2" s="65"/>
+      <c r="U2" s="65"/>
+      <c r="V2" s="65"/>
+      <c r="W2" s="65" t="s">
         <v>154</v>
       </c>
-      <c r="X2" s="66"/>
-      <c r="Y2" s="66"/>
-      <c r="Z2" s="66" t="s">
+      <c r="X2" s="65"/>
+      <c r="Y2" s="65"/>
+      <c r="Z2" s="65" t="s">
         <v>161</v>
       </c>
-      <c r="AA2" s="66"/>
-      <c r="AB2" s="66"/>
-      <c r="AC2" s="66"/>
-      <c r="AD2" s="66"/>
-      <c r="AE2" s="66"/>
-      <c r="AF2" s="66"/>
-      <c r="AG2" s="66"/>
-      <c r="AH2" s="66"/>
-      <c r="AI2" s="66"/>
-      <c r="AJ2" s="66" t="s">
+      <c r="AA2" s="65"/>
+      <c r="AB2" s="65"/>
+      <c r="AC2" s="65"/>
+      <c r="AD2" s="65"/>
+      <c r="AE2" s="65"/>
+      <c r="AF2" s="65"/>
+      <c r="AG2" s="65"/>
+      <c r="AH2" s="65"/>
+      <c r="AI2" s="65"/>
+      <c r="AJ2" s="65" t="s">
         <v>182</v>
       </c>
-      <c r="AK2" s="66"/>
-      <c r="AL2" s="66"/>
-      <c r="AM2" s="66"/>
-      <c r="AN2" s="66"/>
-      <c r="AO2" s="66"/>
-      <c r="AP2" s="66"/>
-      <c r="AQ2" s="66"/>
-      <c r="AR2" s="66"/>
-      <c r="AS2" s="66"/>
+      <c r="AK2" s="65"/>
+      <c r="AL2" s="65"/>
+      <c r="AM2" s="65"/>
+      <c r="AN2" s="65"/>
+      <c r="AO2" s="65"/>
+      <c r="AP2" s="65"/>
+      <c r="AQ2" s="65"/>
+      <c r="AR2" s="65"/>
+      <c r="AS2" s="65"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="68" t="s">
+      <c r="A3" s="67" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="68" t="s">
         <v>111</v>
       </c>
-      <c r="C3" s="56"/>
-      <c r="D3" s="70" t="s">
+      <c r="C3" s="55"/>
+      <c r="D3" s="69" t="s">
         <v>115</v>
       </c>
-      <c r="E3" s="56"/>
-      <c r="F3" s="70" t="s">
+      <c r="E3" s="55"/>
+      <c r="F3" s="69" t="s">
         <v>119</v>
       </c>
-      <c r="G3" s="71" t="s">
+      <c r="G3" s="70" t="s">
         <v>121</v>
       </c>
-      <c r="H3" s="72" t="s">
+      <c r="H3" s="71" t="s">
         <v>44</v>
       </c>
-      <c r="I3" s="72" t="s">
+      <c r="I3" s="71" t="s">
         <v>124</v>
       </c>
-      <c r="J3" s="72" t="s">
+      <c r="J3" s="71" t="s">
         <v>126</v>
       </c>
-      <c r="K3" s="73" t="s">
+      <c r="K3" s="72" t="s">
         <v>128</v>
       </c>
-      <c r="L3" s="71" t="s">
+      <c r="L3" s="70" t="s">
         <v>47</v>
       </c>
-      <c r="M3" s="71" t="s">
+      <c r="M3" s="70" t="s">
         <v>132</v>
       </c>
-      <c r="N3" s="73" t="s">
+      <c r="N3" s="72" t="s">
         <v>134</v>
       </c>
-      <c r="O3" s="72" t="s">
+      <c r="O3" s="71" t="s">
         <v>137</v>
       </c>
-      <c r="P3" s="74" t="s">
+      <c r="P3" s="73" t="s">
         <v>139</v>
       </c>
-      <c r="Q3" s="72" t="s">
+      <c r="Q3" s="71" t="s">
         <v>141</v>
       </c>
-      <c r="R3" s="75" t="s">
+      <c r="R3" s="74" t="s">
         <v>144</v>
       </c>
-      <c r="S3" s="72" t="s">
+      <c r="S3" s="71" t="s">
         <v>146</v>
       </c>
-      <c r="T3" s="72" t="s">
+      <c r="T3" s="71" t="s">
         <v>148</v>
       </c>
-      <c r="U3" s="72" t="s">
+      <c r="U3" s="71" t="s">
         <v>150</v>
       </c>
-      <c r="V3" s="73" t="s">
+      <c r="V3" s="72" t="s">
         <v>152</v>
       </c>
-      <c r="W3" s="75" t="s">
+      <c r="W3" s="74" t="s">
         <v>155</v>
       </c>
-      <c r="X3" s="72" t="s">
+      <c r="X3" s="71" t="s">
         <v>157</v>
       </c>
-      <c r="Y3" s="73" t="s">
+      <c r="Y3" s="72" t="s">
         <v>159</v>
       </c>
-      <c r="Z3" s="75" t="s">
+      <c r="Z3" s="74" t="s">
         <v>162</v>
       </c>
-      <c r="AA3" s="76" t="s">
+      <c r="AA3" s="75" t="s">
         <v>164</v>
       </c>
-      <c r="AB3" s="71" t="s">
+      <c r="AB3" s="70" t="s">
         <v>166</v>
       </c>
-      <c r="AC3" s="72" t="s">
+      <c r="AC3" s="71" t="s">
         <v>168</v>
       </c>
-      <c r="AD3" s="72" t="s">
+      <c r="AD3" s="71" t="s">
         <v>170</v>
       </c>
-      <c r="AE3" s="72" t="s">
+      <c r="AE3" s="71" t="s">
         <v>172</v>
       </c>
-      <c r="AF3" s="72" t="s">
+      <c r="AF3" s="71" t="s">
         <v>174</v>
       </c>
-      <c r="AG3" s="72" t="s">
+      <c r="AG3" s="71" t="s">
         <v>176</v>
       </c>
-      <c r="AH3" s="72" t="s">
+      <c r="AH3" s="71" t="s">
         <v>178</v>
       </c>
-      <c r="AI3" s="73" t="s">
+      <c r="AI3" s="72" t="s">
         <v>180</v>
       </c>
-      <c r="AJ3" s="75" t="s">
+      <c r="AJ3" s="74" t="s">
         <v>183</v>
       </c>
-      <c r="AK3" s="72" t="s">
+      <c r="AK3" s="71" t="s">
         <v>185</v>
       </c>
-      <c r="AL3" s="72" t="s">
+      <c r="AL3" s="71" t="s">
         <v>187</v>
       </c>
-      <c r="AM3" s="72" t="s">
+      <c r="AM3" s="71" t="s">
         <v>189</v>
       </c>
-      <c r="AN3" s="72" t="s">
+      <c r="AN3" s="71" t="s">
         <v>191</v>
       </c>
-      <c r="AO3" s="72" t="s">
+      <c r="AO3" s="71" t="s">
         <v>193</v>
       </c>
-      <c r="AP3" s="72" t="s">
+      <c r="AP3" s="71" t="s">
         <v>195</v>
       </c>
-      <c r="AQ3" s="72" t="s">
+      <c r="AQ3" s="71" t="s">
         <v>197</v>
       </c>
-      <c r="AR3" s="72" t="s">
+      <c r="AR3" s="71" t="s">
         <v>199</v>
       </c>
-      <c r="AS3" s="73" t="s">
+      <c r="AS3" s="72" t="s">
         <v>201</v>
       </c>
-      <c r="AT3" s="77" t="s">
+      <c r="AT3" s="76" t="s">
         <v>203</v>
       </c>
     </row>
@@ -17409,7 +17405,7 @@
       <c r="D4" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="K4" s="78"/>
+      <c r="K4" s="77"/>
       <c r="W4" s="37"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17422,7 +17418,7 @@
       <c r="D5" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="K5" s="78"/>
+      <c r="K5" s="77"/>
       <c r="W5" s="37"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17435,7 +17431,7 @@
       <c r="D6" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="K6" s="78"/>
+      <c r="K6" s="77"/>
       <c r="W6" s="37"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17457,7 +17453,7 @@
       <c r="L7" s="1" t="n">
         <v>9447</v>
       </c>
-      <c r="M7" s="78" t="s">
+      <c r="M7" s="77" t="s">
         <v>224</v>
       </c>
       <c r="P7" s="1" t="s">
@@ -17466,8 +17462,11 @@
       <c r="V7" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="AA7" s="79" t="s">
+      <c r="AA7" s="78" t="s">
         <v>227</v>
+      </c>
+      <c r="AB7" s="40" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22526,7 +22525,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="153.83"/>
@@ -22545,15 +22544,15 @@
         <v>71</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="34" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove non-vcf files from metadata
</commit_message>
<xml_diff>
--- a/tests/resources/EVA_Submission_test.xlsx
+++ b/tests/resources/EVA_Submission_test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="PLEASE READ FIRST" sheetId="1" state="visible" r:id="rId3"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="593">
   <si>
     <t xml:space="preserve">PLEASE READ FIRST</t>
   </si>
@@ -968,6 +968,9 @@
   </si>
   <si>
     <t xml:space="preserve">example3.vcf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">example2.vcf.gz.tbi</t>
   </si>
   <si>
     <t xml:space="preserve">Sample(s)</t>
@@ -3038,7 +3041,7 @@
   </sheetPr>
   <dimension ref="A1:AMK23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -7360,8 +7363,8 @@
   </sheetPr>
   <dimension ref="A1:B1001"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7403,7 +7406,12 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="42"/>
+      <c r="A5" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="42"/>
@@ -10399,7 +10407,7 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Must match an analysis alias provided in the &quot;ANALYSIS&quot; sheet&#10;Multiple entries can be separated with a comma&#10;e.g. analysis1,analysis2" promptTitle="Analysis alias" showDropDown="false" showErrorMessage="false" showInputMessage="true" sqref="A5:A1001" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Must match an analysis alias provided in the &quot;ANALYSIS&quot; sheet&#10;Multiple entries can be separated with a comma&#10;e.g. analysis1,analysis2" promptTitle="Analysis alias" showDropDown="false" showErrorMessage="false" showInputMessage="true" sqref="A6:A1001" type="list">
       <formula1>Analysis!$B$2:$B$100000</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -10435,7 +10443,7 @@
   <sheetData>
     <row r="1" s="54" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="82" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D1" s="82" t="s">
         <v>16</v>
@@ -10466,229 +10474,229 @@
         <v>109</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="F3" s="83"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B4" s="42" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B5" s="42" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B6" s="42" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B7" s="42" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B8" s="42" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B9" s="42" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B10" s="42" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B11" s="42" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B12" s="42" t="s">
+        <v>278</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>276</v>
-      </c>
-      <c r="B12" s="42" t="s">
-        <v>277</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="42" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="42" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="42" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="42" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="42" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="42" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="42" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="42" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="42" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="42" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="42" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="42" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="42" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>112</v>
@@ -10696,1392 +10704,1392 @@
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="42" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="42" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="42" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="42" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="42" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="42" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="42" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="42" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="42" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="42" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="42" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="42" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="42" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="42" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="42" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="42" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="42" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="42" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="42" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="42" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="42" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="42" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="42" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="42" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="42" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="42" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="42" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="42" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="42" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="42" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="E55" s="54"/>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="42" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="42" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="42" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="42" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="42" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="42" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="42" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="42" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="42" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="42" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="42" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="42" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="42" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="42" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="42" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="42" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="42" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="42" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="42" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="42" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="42" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="42" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="42" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="42" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="42" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="42" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="42" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="42" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="42" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="42" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="42" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="42" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="42" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="42" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="42" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="42" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="42" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B93" s="42" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="42" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="42" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="42" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="42" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="42" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="42" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="42" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="42" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="42" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="42" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="42" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="42" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="42" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="42" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="42" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="42" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B110" s="42" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B111" s="42" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="42" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="42" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="42" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="42" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B116" s="42" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B117" s="42" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="42" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B119" s="42" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="42" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B121" s="42" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="42" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="42" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="42" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="42" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B126" s="42" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B127" s="42" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B128" s="42" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B129" s="42" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B130" s="42" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B131" s="42" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B132" s="42" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B133" s="42" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B134" s="42" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B135" s="42" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B136" s="42" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B137" s="42" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B138" s="42" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B139" s="42" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B140" s="42" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B141" s="42" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B142" s="42" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B143" s="42" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B144" s="42" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B145" s="42" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B146" s="42" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B147" s="42" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B148" s="42" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B149" s="42" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B150" s="42" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B151" s="42" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B152" s="42" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B153" s="42" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B154" s="42" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B155" s="42" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B156" s="42" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B157" s="42" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B158" s="42" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B159" s="42" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B160" s="42" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B161" s="42" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B162" s="42" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B163" s="42" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B164" s="42" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B165" s="42" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B166" s="42" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B167" s="42" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B168" s="42" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B169" s="42" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B170" s="42" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B171" s="42" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B172" s="42" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B173" s="42" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B174" s="42" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B175" s="42" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B176" s="42" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B177" s="42" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B178" s="42" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B179" s="42" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B180" s="42" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B181" s="42" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B182" s="42" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B183" s="42" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B184" s="42" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B185" s="42" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B186" s="42" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B187" s="42" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B188" s="42" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B189" s="42" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B190" s="42" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B191" s="42" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B192" s="42" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B193" s="42" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B194" s="42" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B195" s="42" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B196" s="42" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B197" s="42" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B198" s="42" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B199" s="42" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B200" s="42" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B201" s="42" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B202" s="42" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B203" s="42" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B204" s="42" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B205" s="42" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B206" s="42" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B207" s="42" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B208" s="42" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B209" s="42" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B210" s="42" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B211" s="42" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B212" s="42" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B213" s="42" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B214" s="42" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B215" s="42" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B216" s="42" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B217" s="42" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B218" s="42" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B219" s="42" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B220" s="42" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B221" s="42" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B222" s="42" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B223" s="42" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B224" s="42" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B225" s="42" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B226" s="42" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B227" s="42" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B228" s="42" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B229" s="42" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B230" s="42" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B231" s="42" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B232" s="42" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B233" s="42" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B234" s="42" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B235" s="42" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B236" s="42" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B237" s="42" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B238" s="42" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B239" s="42" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B240" s="42" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B241" s="42" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B242" s="42" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B243" s="42" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B244" s="42" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B245" s="42" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B246" s="42" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B247" s="42" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B248" s="42" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B249" s="42" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B250" s="42" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B251" s="42" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B252" s="42" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B253" s="42" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B254" s="42" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B255" s="42" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B256" s="42" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B257" s="42" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B258" s="42" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B259" s="42" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B260" s="42" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B261" s="42" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B262" s="42" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B263" s="42" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B264" s="42" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B265" s="42" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B266" s="42" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B267" s="42" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B268" s="42" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B269" s="42" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B270" s="42" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B271" s="42" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B272" s="42" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B273" s="42" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B274" s="42" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B275" s="42" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B276" s="42" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B277" s="42" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B278" s="42" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B279" s="42" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B280" s="42" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B281" s="42" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B282" s="42" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B283" s="84" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B284" s="84" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B285" s="84" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B286" s="84" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
     </row>
   </sheetData>

</xml_diff>